<commit_message>
finishing up last figures
</commit_message>
<xml_diff>
--- a/Cu_shielding_meas/sheilding_meas_12-6.xlsx
+++ b/Cu_shielding_meas/sheilding_meas_12-6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandraklipfel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandraklipfel/Desktop/senior_thesis/Cu_shielding_meas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151ECF21-6A48-4140-9FD3-393678CFD8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8A64E-AD59-CF44-A93E-FD3EF675BC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="3060" windowWidth="31900" windowHeight="15940" xr2:uid="{7A881133-112B-B540-A9CF-5BE9FCF47A3C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31900" windowHeight="15940" xr2:uid="{7A881133-112B-B540-A9CF-5BE9FCF47A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,6 +168,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -177,12 +183,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,12 +243,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Pick-up Voltage</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37563435702228098"/>
+          <c:y val="5.7934621954660107E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -280,7 +288,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9433259902323365E-2"/>
+          <c:y val="0.15721424651304458"/>
+          <c:w val="0.67180311487695699"/>
+          <c:h val="0.65820313193954416"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -567,12 +585,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Frequency (Hz)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.3600719088263965"/>
+              <c:y val="0.85596772223945561"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -687,7 +713,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Pick-up Voltage (mV)</a:t>
                 </a:r>
               </a:p>
@@ -767,6 +793,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76599896389183519"/>
+          <c:y val="0.35274398238257365"/>
+          <c:w val="0.226199510203413"/>
+          <c:h val="0.23379792971078911"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -874,12 +910,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Phase</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46468638018027741"/>
+          <c:y val="2.7065387418644001E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -911,7 +955,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10490353656501628"/>
+          <c:y val="0.12570642211077473"/>
+          <c:w val="0.70094600810277652"/>
+          <c:h val="0.76060655141241806"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1198,7 +1252,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Frequency (Hz)</a:t>
                 </a:r>
               </a:p>
@@ -1318,7 +1372,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Phase (deg.)</a:t>
                 </a:r>
               </a:p>
@@ -2593,10 +2647,10 @@
       <xdr:rowOff>46830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1398840</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>128840</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>925061</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>31358</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2625,14 +2679,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>581854</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50649</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1435651</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>18405</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>925794</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>272990</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2959,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D97E4D7-4908-024A-A666-B45DD035422B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="89" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="F17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2969,378 +3023,378 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="6">
         <v>10</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="6">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="6">
         <v>1E-4</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="6">
         <v>85.7</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="6">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="6">
         <v>100</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <v>1E-4</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="6">
         <v>73.66</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="6">
         <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="6">
         <v>500</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>0.17649999999999999</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="6">
         <v>72.3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="6">
         <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="6">
         <v>1000</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>0.32600000000000001</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>64.599999999999994</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="6">
         <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="6">
         <v>5000</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>1.2030000000000001</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="6">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <v>-64</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="6">
         <v>2</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="6">
         <v>7500</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>1.1200000000000001</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>0.01</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>-149</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="6">
         <v>2</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="6">
         <v>10000</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="6">
         <v>0.94140000000000001</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>-178.29</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="6">
         <v>0.01</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="6">
         <v>20000</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>2.75E-2</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6">
         <v>104</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="A14" s="4">
         <v>2</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <v>1E-4</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>85.3</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <v>0.04</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="4">
         <v>100</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="4">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>1E-4</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>73.599999999999994</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="A16" s="4">
         <v>2</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>500</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>0.1779</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>1E-4</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>73.3</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="4">
         <v>0.06</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>2</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>1000</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>0.32919999999999999</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>1E-3</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>66.5</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>5000</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>1.31</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <v>0.01</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>-58</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="A19" s="4">
         <v>2</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>7500</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>1.4</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>0.1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>-134.5</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="A20" s="4">
         <v>2</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>10000</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>0.01</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>-170</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="A21" s="4">
         <v>2</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>20000</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>0.04</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>1E-3</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>103.2</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>